<commit_message>
Add CPU & SA test bench
(1) find a CPU debug when use SUIH instruction;
(2) modify top level module and change IO control bits;
(3) the testbench finish logic of BPF, save data to D_MEM, but something
wrong with the super ALU
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F6:G30"/>
+  <dimension ref="F6:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +578,686 @@
         <v>34</v>
       </c>
     </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="143" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="144" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="146" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="148" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="149" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="150" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="151" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="152" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="155" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="157" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="158" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="159" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="162" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="163" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="164" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="166" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish ALU_CTRL_SPI module and the top level module
(1) ALU_CTRL_SPI module and the top level module compile successfully;
(2) remove the unnecessary comments from codes;
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -4,13 +4,175 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pad_name" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+  <si>
+    <t xml:space="preserve">    PIC     ipad_adc_pi0    (.Y(i_ADC_PI[0]), .P(ADC_PI[0]), .IE(1'b1));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PIC     ipad_adc_pi1    (.Y(i_ADC_PI[1]), .P(ADC_PI[1]), .IE(1'b1));</t>
+  </si>
+  <si>
+    <t>PIC</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi0</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi1</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[0</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[1</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[0</t>
+  </si>
+  <si>
+    <t>]), .IE(1'b1));</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[1</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi2</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[2</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[2</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi3</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[3</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[3</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi4</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[4</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[4</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi5</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[5</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[5</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi6</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[6</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[6</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi7</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[7</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[7</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi8</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[8</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[8</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi9</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[9</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[9</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi10</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[10</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[10</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi11</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[11</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[11</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi12</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[12</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[12</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi13</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[13</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[13</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi14</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[14</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[14</t>
+  </si>
+  <si>
+    <t>ipad_adc_pi15</t>
+  </si>
+  <si>
+    <t>(.Y(i_ADC_PI[15</t>
+  </si>
+  <si>
+    <t>]), .P(ADC_PI[15</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
@@ -1261,4 +1423,307 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
debug the SA instructions module
(1) add the wait instructions in SA module; (2) modify the testbench
file; (3) enlarge the scan chain length from 13 to 32 by using excel;
(4) still some bugs in the SA instructions module and the testbench;
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="pad_name" sheetId="2" r:id="rId2"/>
+    <sheet name="fpga_sc" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
   <si>
     <t xml:space="preserve">    PIC     ipad_adc_pi0    (.Y(i_ADC_PI[0]), .P(ADC_PI[0]), .IE(1'b1));</t>
   </si>
@@ -171,6 +172,240 @@
   </si>
   <si>
     <t>]), .P(ADC_PI[15</t>
+  </si>
+  <si>
+    <t>SC_CELL_V3</t>
+  </si>
+  <si>
+    <t>( .SIN(</t>
+  </si>
+  <si>
+    <t>), .SO(</t>
+  </si>
+  <si>
+    <t>), .PO(</t>
+  </si>
+  <si>
+    <t>), .PIN(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .BYP_N(</t>
+  </si>
+  <si>
+    <t>1'b0</t>
+  </si>
+  <si>
+    <t>) );</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>CS208</t>
+  </si>
+  <si>
+    <t>M0</t>
+  </si>
+  <si>
+    <t>CS209</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>CS210</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>CS211</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>CS212</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>CS213</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>CS214</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>CS215</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>CS216</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>CS217</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>CS218</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>CS219</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>CS220</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>CS221</t>
+  </si>
+  <si>
+    <t>SO_B</t>
+  </si>
+  <si>
+    <t>CS222</t>
+  </si>
+  <si>
+    <t>CS223</t>
+  </si>
+  <si>
+    <t>CS224</t>
+  </si>
+  <si>
+    <t>CS225</t>
+  </si>
+  <si>
+    <t>CS226</t>
+  </si>
+  <si>
+    <t>CS227</t>
+  </si>
+  <si>
+    <t>CS228</t>
+  </si>
+  <si>
+    <t>CS229</t>
+  </si>
+  <si>
+    <t>CS230</t>
+  </si>
+  <si>
+    <t>CS231</t>
+  </si>
+  <si>
+    <t>CS232</t>
+  </si>
+  <si>
+    <t>CS233</t>
+  </si>
+  <si>
+    <t>CS234</t>
+  </si>
+  <si>
+    <t>CS235</t>
+  </si>
+  <si>
+    <t>CS236</t>
+  </si>
+  <si>
+    <t>CS237</t>
+  </si>
+  <si>
+    <t>CS238</t>
+  </si>
+  <si>
+    <t>CS239</t>
+  </si>
+  <si>
+    <t>SPI_SO_dly</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>M17</t>
+  </si>
+  <si>
+    <t>M18</t>
+  </si>
+  <si>
+    <t>M19</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>M21</t>
+  </si>
+  <si>
+    <t>M22</t>
+  </si>
+  <si>
+    <t>M23</t>
+  </si>
+  <si>
+    <t>M24</t>
+  </si>
+  <si>
+    <t>M25</t>
+  </si>
+  <si>
+    <t>M26</t>
+  </si>
+  <si>
+    <t>M27</t>
+  </si>
+  <si>
+    <t>M28</t>
+  </si>
+  <si>
+    <t>M29</t>
+  </si>
+  <si>
+    <t>M30</t>
+  </si>
+  <si>
+    <t>CFSA_FOUT</t>
+  </si>
+  <si>
+    <t>FOUT</t>
+  </si>
+  <si>
+    <t>), .SEL(SEL_B), .LAT(LAT_dly), .SCK1(SCLK1_dly), .SCK2(SCLK2_dly),</t>
   </si>
 </sst>
 </file>
@@ -214,74 +449,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -301,7 +468,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CFE4CD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1429,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:F22"/>
     </sheetView>
   </sheetViews>
@@ -1726,4 +1893,2017 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:U49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="1.28515625" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
+        <v>129</v>
+      </c>
+      <c r="S2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
+        <v>129</v>
+      </c>
+      <c r="S3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>129</v>
+      </c>
+      <c r="S4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" t="s">
+        <v>128</v>
+      </c>
+      <c r="O5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
+        <v>129</v>
+      </c>
+      <c r="S5" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>128</v>
+      </c>
+      <c r="O6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" t="s">
+        <v>129</v>
+      </c>
+      <c r="S6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" t="s">
+        <v>128</v>
+      </c>
+      <c r="O7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7">
+        <v>26</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" t="s">
+        <v>129</v>
+      </c>
+      <c r="S7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7" t="s">
+        <v>58</v>
+      </c>
+      <c r="U7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" t="s">
+        <v>128</v>
+      </c>
+      <c r="O8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8" t="s">
+        <v>129</v>
+      </c>
+      <c r="S8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" t="s">
+        <v>128</v>
+      </c>
+      <c r="O9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P9">
+        <v>24</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" t="s">
+        <v>129</v>
+      </c>
+      <c r="S9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s">
+        <v>128</v>
+      </c>
+      <c r="O10" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10">
+        <v>23</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>61</v>
+      </c>
+      <c r="R10" t="s">
+        <v>129</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T10" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" t="s">
+        <v>129</v>
+      </c>
+      <c r="S11" t="s">
+        <v>57</v>
+      </c>
+      <c r="T11" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" t="s">
+        <v>128</v>
+      </c>
+      <c r="O12" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12">
+        <v>21</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12" t="s">
+        <v>129</v>
+      </c>
+      <c r="S12" t="s">
+        <v>57</v>
+      </c>
+      <c r="T12" t="s">
+        <v>58</v>
+      </c>
+      <c r="U12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13">
+        <v>20</v>
+      </c>
+      <c r="L13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" t="s">
+        <v>128</v>
+      </c>
+      <c r="O13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" t="s">
+        <v>129</v>
+      </c>
+      <c r="S13" t="s">
+        <v>57</v>
+      </c>
+      <c r="T13" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14">
+        <v>19</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" t="s">
+        <v>128</v>
+      </c>
+      <c r="O14" t="s">
+        <v>60</v>
+      </c>
+      <c r="P14">
+        <v>19</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R14" t="s">
+        <v>129</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" t="s">
+        <v>58</v>
+      </c>
+      <c r="U14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15">
+        <v>18</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15">
+        <v>18</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>129</v>
+      </c>
+      <c r="S15" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15" t="s">
+        <v>58</v>
+      </c>
+      <c r="U15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>17</v>
+      </c>
+      <c r="L16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" t="s">
+        <v>128</v>
+      </c>
+      <c r="O16" t="s">
+        <v>60</v>
+      </c>
+      <c r="P16">
+        <v>17</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>61</v>
+      </c>
+      <c r="R16" t="s">
+        <v>129</v>
+      </c>
+      <c r="S16" t="s">
+        <v>57</v>
+      </c>
+      <c r="T16" t="s">
+        <v>58</v>
+      </c>
+      <c r="U16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" t="s">
+        <v>128</v>
+      </c>
+      <c r="O17" t="s">
+        <v>60</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R17" t="s">
+        <v>129</v>
+      </c>
+      <c r="S17" t="s">
+        <v>57</v>
+      </c>
+      <c r="T17" t="s">
+        <v>58</v>
+      </c>
+      <c r="U17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18">
+        <v>15</v>
+      </c>
+      <c r="L18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" t="s">
+        <v>128</v>
+      </c>
+      <c r="O18" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18">
+        <v>15</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>61</v>
+      </c>
+      <c r="R18" t="s">
+        <v>129</v>
+      </c>
+      <c r="S18" t="s">
+        <v>57</v>
+      </c>
+      <c r="T18" t="s">
+        <v>58</v>
+      </c>
+      <c r="U18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>128</v>
+      </c>
+      <c r="O19" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19">
+        <v>14</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>61</v>
+      </c>
+      <c r="R19" t="s">
+        <v>129</v>
+      </c>
+      <c r="S19" t="s">
+        <v>57</v>
+      </c>
+      <c r="T19" t="s">
+        <v>58</v>
+      </c>
+      <c r="U19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" t="s">
+        <v>128</v>
+      </c>
+      <c r="O20" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20">
+        <v>13</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>61</v>
+      </c>
+      <c r="R20" t="s">
+        <v>129</v>
+      </c>
+      <c r="S20" t="s">
+        <v>57</v>
+      </c>
+      <c r="T20" t="s">
+        <v>58</v>
+      </c>
+      <c r="U20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21">
+        <v>12</v>
+      </c>
+      <c r="L21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" t="s">
+        <v>128</v>
+      </c>
+      <c r="O21" t="s">
+        <v>60</v>
+      </c>
+      <c r="P21">
+        <v>12</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>61</v>
+      </c>
+      <c r="R21" t="s">
+        <v>129</v>
+      </c>
+      <c r="S21" t="s">
+        <v>57</v>
+      </c>
+      <c r="T21" t="s">
+        <v>58</v>
+      </c>
+      <c r="U21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" t="s">
+        <v>127</v>
+      </c>
+      <c r="J22" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22" t="s">
+        <v>61</v>
+      </c>
+      <c r="M22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" t="s">
+        <v>128</v>
+      </c>
+      <c r="O22" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>61</v>
+      </c>
+      <c r="R22" t="s">
+        <v>129</v>
+      </c>
+      <c r="S22" t="s">
+        <v>57</v>
+      </c>
+      <c r="T22" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" t="s">
+        <v>128</v>
+      </c>
+      <c r="O23" t="s">
+        <v>60</v>
+      </c>
+      <c r="P23">
+        <v>10</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>61</v>
+      </c>
+      <c r="R23" t="s">
+        <v>129</v>
+      </c>
+      <c r="S23" t="s">
+        <v>57</v>
+      </c>
+      <c r="T23" t="s">
+        <v>58</v>
+      </c>
+      <c r="U23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>61</v>
+      </c>
+      <c r="R24" t="s">
+        <v>129</v>
+      </c>
+      <c r="S24" t="s">
+        <v>57</v>
+      </c>
+      <c r="T24" t="s">
+        <v>58</v>
+      </c>
+      <c r="U24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" t="s">
+        <v>56</v>
+      </c>
+      <c r="N25" t="s">
+        <v>128</v>
+      </c>
+      <c r="O25" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25">
+        <v>8</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>61</v>
+      </c>
+      <c r="R25" t="s">
+        <v>129</v>
+      </c>
+      <c r="S25" t="s">
+        <v>57</v>
+      </c>
+      <c r="T25" t="s">
+        <v>58</v>
+      </c>
+      <c r="U25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" t="s">
+        <v>60</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" t="s">
+        <v>128</v>
+      </c>
+      <c r="O26" t="s">
+        <v>60</v>
+      </c>
+      <c r="P26">
+        <v>7</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>61</v>
+      </c>
+      <c r="R26" t="s">
+        <v>129</v>
+      </c>
+      <c r="S26" t="s">
+        <v>57</v>
+      </c>
+      <c r="T26" t="s">
+        <v>58</v>
+      </c>
+      <c r="U26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27">
+        <v>6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" t="s">
+        <v>128</v>
+      </c>
+      <c r="O27" t="s">
+        <v>60</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>61</v>
+      </c>
+      <c r="R27" t="s">
+        <v>129</v>
+      </c>
+      <c r="S27" t="s">
+        <v>57</v>
+      </c>
+      <c r="T27" t="s">
+        <v>58</v>
+      </c>
+      <c r="U27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" t="s">
+        <v>128</v>
+      </c>
+      <c r="O28" t="s">
+        <v>60</v>
+      </c>
+      <c r="P28">
+        <v>5</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>61</v>
+      </c>
+      <c r="R28" t="s">
+        <v>129</v>
+      </c>
+      <c r="S28" t="s">
+        <v>57</v>
+      </c>
+      <c r="T28" t="s">
+        <v>58</v>
+      </c>
+      <c r="U28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J29" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" t="s">
+        <v>128</v>
+      </c>
+      <c r="O29" t="s">
+        <v>60</v>
+      </c>
+      <c r="P29">
+        <v>4</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>61</v>
+      </c>
+      <c r="R29" t="s">
+        <v>129</v>
+      </c>
+      <c r="S29" t="s">
+        <v>57</v>
+      </c>
+      <c r="T29" t="s">
+        <v>58</v>
+      </c>
+      <c r="U29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" t="s">
+        <v>127</v>
+      </c>
+      <c r="J30" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" t="s">
+        <v>56</v>
+      </c>
+      <c r="N30" t="s">
+        <v>128</v>
+      </c>
+      <c r="O30" t="s">
+        <v>60</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>61</v>
+      </c>
+      <c r="R30" t="s">
+        <v>129</v>
+      </c>
+      <c r="S30" t="s">
+        <v>57</v>
+      </c>
+      <c r="T30" t="s">
+        <v>58</v>
+      </c>
+      <c r="U30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" t="s">
+        <v>60</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="N31" t="s">
+        <v>128</v>
+      </c>
+      <c r="O31" t="s">
+        <v>60</v>
+      </c>
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>61</v>
+      </c>
+      <c r="R31" t="s">
+        <v>129</v>
+      </c>
+      <c r="S31" t="s">
+        <v>57</v>
+      </c>
+      <c r="T31" t="s">
+        <v>58</v>
+      </c>
+      <c r="U31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" t="s">
+        <v>56</v>
+      </c>
+      <c r="N32" t="s">
+        <v>128</v>
+      </c>
+      <c r="O32" t="s">
+        <v>60</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>61</v>
+      </c>
+      <c r="R32" t="s">
+        <v>129</v>
+      </c>
+      <c r="S32" t="s">
+        <v>57</v>
+      </c>
+      <c r="T32" t="s">
+        <v>58</v>
+      </c>
+      <c r="U32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" t="s">
+        <v>127</v>
+      </c>
+      <c r="J33" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" t="s">
+        <v>128</v>
+      </c>
+      <c r="O33" t="s">
+        <v>60</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>61</v>
+      </c>
+      <c r="R33" t="s">
+        <v>129</v>
+      </c>
+      <c r="S33" t="s">
+        <v>57</v>
+      </c>
+      <c r="T33" t="s">
+        <v>58</v>
+      </c>
+      <c r="U33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>